<commit_message>
no b and b now independant
</commit_message>
<xml_diff>
--- a/sampledata.xlsx
+++ b/sampledata.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\Programming&amp;Coding\VS Code Projects\2VariableLinearLeastSquaresFit&amp;Plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCDB0C3-3214-4F22-BB69-A83CB520DDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD636E12-0941-41A9-84A0-4A575F3EF7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15540" yWindow="-2415" windowWidth="15330" windowHeight="8610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17025" yWindow="-3465" windowWidth="15330" windowHeight="8610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,13 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
-  <si>
-    <t>1/i</t>
-  </si>
-  <si>
-    <t>1/p</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>di</t>
   </si>
@@ -443,11 +437,247 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A254C8-768D-4054-BF61-A15B46BEA4C0}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0.22883295200000001</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-0.25706940900000003</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.618226E-3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3.3042340000000001E-3</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>0.23696682499999999</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-0.25706940900000003</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.8076640000000001E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3.3042340000000001E-3</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>-4.2034467999999998E-2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.7889088000000001E-2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>8.8344799999999995E-5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.6001000000000001E-5</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>-4.6948357000000003E-2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.9794141000000001E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.10207E-4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.9590400000000001E-5</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>-3.5460993000000003E-2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.1466575E-2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>6.2874100000000002E-5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>6.57412E-6</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>-4.2176297000000001E-2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.5489467E-2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>8.8942000000000003E-5</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1.19962E-5</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>-4.2936883000000002E-2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.8552875999999999E-2</v>
+      </c>
+      <c r="C8" s="5">
+        <v>9.2178799999999999E-5</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1.7210500000000001E-5</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>-4.2176297000000001E-2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.7298045000000001E-2</v>
+      </c>
+      <c r="C9" s="5">
+        <v>8.8942000000000003E-5</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1.49611E-5</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>-4.6620046999999998E-2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2.0218357999999999E-2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.08671E-4</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2.0439099999999999E-5</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>-5.0226016999999998E-2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2.4265954999999999E-2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.2613300000000001E-4</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2.94418E-5</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>-5.5279160000000001E-2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.9377203000000001E-2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.5278899999999999E-4</v>
+      </c>
+      <c r="D12" s="5">
+        <v>4.3151000000000001E-5</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>-7.8740157000000005E-2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3.7023325000000003E-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3.1000100000000002E-4</v>
+      </c>
+      <c r="D13" s="5">
+        <v>6.8536300000000003E-5</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G16" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F21624E-331F-4DA1-9A54-5A26E501B9A0}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,16 +690,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -809,240 +1039,6 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A254C8-768D-4054-BF61-A15B46BEA4C0}">
-  <dimension ref="A1:H16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>0.22883295200000001</v>
-      </c>
-      <c r="B2" s="2">
-        <v>-0.25706940900000003</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2.618226E-3</v>
-      </c>
-      <c r="D2" s="2">
-        <v>3.3042340000000001E-3</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>0.23696682499999999</v>
-      </c>
-      <c r="B3" s="2">
-        <v>-0.25706940900000003</v>
-      </c>
-      <c r="C3" s="2">
-        <v>2.8076640000000001E-3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>3.3042340000000001E-3</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>-4.2034467999999998E-2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1.7889088000000001E-2</v>
-      </c>
-      <c r="C4" s="5">
-        <v>8.8344799999999995E-5</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1.6001000000000001E-5</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>-4.6948357000000003E-2</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1.9794141000000001E-2</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.10207E-4</v>
-      </c>
-      <c r="D5" s="5">
-        <v>1.9590400000000001E-5</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>-3.5460993000000003E-2</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1.1466575E-2</v>
-      </c>
-      <c r="C6" s="5">
-        <v>6.2874100000000002E-5</v>
-      </c>
-      <c r="D6" s="5">
-        <v>6.57412E-6</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>-4.2176297000000001E-2</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1.5489467E-2</v>
-      </c>
-      <c r="C7" s="5">
-        <v>8.8942000000000003E-5</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1.19962E-5</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>-4.2936883000000002E-2</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1.8552875999999999E-2</v>
-      </c>
-      <c r="C8" s="5">
-        <v>9.2178799999999999E-5</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.7210500000000001E-5</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>-4.2176297000000001E-2</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1.7298045000000001E-2</v>
-      </c>
-      <c r="C9" s="5">
-        <v>8.8942000000000003E-5</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1.49611E-5</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>-4.6620046999999998E-2</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2.0218357999999999E-2</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.08671E-4</v>
-      </c>
-      <c r="D10" s="5">
-        <v>2.0439099999999999E-5</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>-5.0226016999999998E-2</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2.4265954999999999E-2</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1.2613300000000001E-4</v>
-      </c>
-      <c r="D11" s="5">
-        <v>2.94418E-5</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>-5.5279160000000001E-2</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2.9377203000000001E-2</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1.5278899999999999E-4</v>
-      </c>
-      <c r="D12" s="5">
-        <v>4.3151000000000001E-5</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>-7.8740157000000005E-2</v>
-      </c>
-      <c r="B13" s="2">
-        <v>3.7023325000000003E-2</v>
-      </c>
-      <c r="C13" s="2">
-        <v>3.1000100000000002E-4</v>
-      </c>
-      <c r="D13" s="5">
-        <v>6.8536300000000003E-5</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>